<commit_message>
Added  FolderManager::ComputeParentFolderSize, more test cases
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPMENT\PROJECTs\Visual Studio 2022\FindIt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B0EA5-C677-400D-8CE0-0DDBE2B1102E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A08C86-9172-4847-B5AF-AE6E11C022F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="2256" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="C.Users.acarz" sheetId="5" r:id="rId1"/>
-    <sheet name="C.Users.All Users" sheetId="1" r:id="rId2"/>
-    <sheet name="C.Users.Public" sheetId="2" r:id="rId3"/>
-    <sheet name="C.Users.Default" sheetId="3" r:id="rId4"/>
-    <sheet name="C.Program Files (x86)" sheetId="4" r:id="rId5"/>
+    <sheet name="C.Users" sheetId="6" r:id="rId1"/>
+    <sheet name="C.Users.acarz" sheetId="5" r:id="rId2"/>
+    <sheet name="C.Users.All Users" sheetId="1" r:id="rId3"/>
+    <sheet name="C.Users.Public" sheetId="2" r:id="rId4"/>
+    <sheet name="C.Users.Default" sheetId="3" r:id="rId5"/>
+    <sheet name="C.Program Files (x86)" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>C:\users\all users : this is an alias to:  C:\ProgramData</t>
   </si>
@@ -155,6 +156,48 @@
   </si>
   <si>
     <t>Size matches Windows explorer reported size</t>
+  </si>
+  <si>
+    <t>Before: 2025-04-07 02:06:53</t>
+  </si>
+  <si>
+    <t>After: 2025-04-07 02:07:42 Folder size: 233462132864</t>
+  </si>
+  <si>
+    <t>After2: 2025-04-07 02:07:42</t>
+  </si>
+  <si>
+    <t>Number of files: 13</t>
+  </si>
+  <si>
+    <t>After3: 2025-04-07 02:07:42</t>
+  </si>
+  <si>
+    <t>Folder C:\Users\acarz size: 233462132864 last checked: 1969-12-31 23:59:59 last modified: 1969-12-31 23:59:59</t>
+  </si>
+  <si>
+    <t>Folders::GetInstance().ComputeFolderSizeInternally("C:\\Users\\acarz");</t>
+  </si>
+  <si>
+    <t>Windows explorer shows 284,193,604,168</t>
+  </si>
+  <si>
+    <t>Before: 2025-04-07 02:35:54</t>
+  </si>
+  <si>
+    <t>After: 2025-04-07 02:37:07 Folder size: 275836550185</t>
+  </si>
+  <si>
+    <t>After2: 2025-04-07 02:37:07</t>
+  </si>
+  <si>
+    <t>After3: 2025-04-07 02:37:07</t>
+  </si>
+  <si>
+    <t>Folder C:\Users\acarz size: 275836550185 last checked: 1969-12-31 23:59:59 last modified: 1969-12-31 23:59:59</t>
+  </si>
+  <si>
+    <t>executed as admin :</t>
   </si>
 </sst>
 </file>
@@ -490,11 +533,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEB0550-F1F2-4D68-8AAB-97C08426F5C6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5966FF6-B853-452E-A192-287202020808}">
-  <dimension ref="A3:E14"/>
+  <dimension ref="A3:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -574,12 +629,93 @@
         <v>31</v>
       </c>
     </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2"/>
   <sheetViews>
@@ -599,7 +735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B5B21F-916C-4A19-B088-40D311B17303}">
   <dimension ref="A3:C13"/>
   <sheetViews>
@@ -678,12 +814,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A85F582-FB31-49E7-9D0B-452EBEAEC4A1}">
   <dimension ref="A3:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -778,7 +914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC95C6D-6FC6-405F-A0AE-5287B445F7A6}">
   <dimension ref="A3:D15"/>
   <sheetViews>

</xml_diff>